<commit_message>
All staff Data set unique id
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/002.xlsx
+++ b/docs/STAFF-DATA/002.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai_Vignesh\Desktop\002_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1E981D-FB26-450D-9D84-134EE8DDAED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="13900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,16 +159,19 @@
     <t>VEC-002-04-160</t>
   </si>
   <si>
-    <t>VEC-002-03-167</t>
-  </si>
-  <si>
     <t>www.linkedin.com/in/jemima-chandra-d-s-b34586184</t>
+  </si>
+  <si>
+    <t>VEC-002-04-167</t>
+  </si>
+  <si>
+    <t>VEC-002-03-168</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -258,9 +260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,9 +300,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,7 +337,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,7 +372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,16 +545,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+    <col min="9" max="9" width="47.08984375" customWidth="1"/>
+    <col min="10" max="10" width="44.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -607,10 +614,10 @@
         <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -642,7 +649,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -674,7 +681,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -703,10 +710,10 @@
         <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -714,32 +721,35 @@
         <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="I3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="H4" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="I4" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D5" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E5" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H5" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="I6" r:id="rId21" xr:uid="{558EC049-8D2D-461A-BEAA-AA870B917CC1}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId6"/>
+    <hyperlink ref="G3" r:id="rId7"/>
+    <hyperlink ref="H3" r:id="rId8"/>
+    <hyperlink ref="I3" r:id="rId9"/>
+    <hyperlink ref="D4" r:id="rId10"/>
+    <hyperlink ref="E4" r:id="rId11"/>
+    <hyperlink ref="F4" r:id="rId12"/>
+    <hyperlink ref="G4" r:id="rId13"/>
+    <hyperlink ref="H4" r:id="rId14"/>
+    <hyperlink ref="I4" r:id="rId15"/>
+    <hyperlink ref="D5" r:id="rId16"/>
+    <hyperlink ref="E5" r:id="rId17"/>
+    <hyperlink ref="F5" r:id="rId18"/>
+    <hyperlink ref="G5" r:id="rId19"/>
+    <hyperlink ref="H5" r:id="rId20"/>
+    <hyperlink ref="I6" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
all name changes and coe added
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/002.xlsx
+++ b/docs/STAFF-DATA/002.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF65F13-527A-4440-8149-229E29BC50BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -46,128 +52,136 @@
     <t>unique_id</t>
   </si>
   <si>
-    <t>Dr. V.Chandran, M.Tech., PhD</t>
+    <t>Dr. BASKARA SETHUPATHY S</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Dr. CHANDRAN V</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/V-Chandran?ev=hdr_xprf</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/sources.uri?zone=TopNavBar&amp;origin=searchauthorfreelookup</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dr-v-chandran-b54505117/</t>
+  </si>
+  <si>
+    <t>VEC-002-03-168</t>
+  </si>
+  <si>
+    <t>JEMIMA CHANDRA D S</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/002/VEC-002-04-002.webp</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/jemima-chandra-d-s-b34586184</t>
+  </si>
+  <si>
+    <t>VEC-002-04-002</t>
+  </si>
+  <si>
+    <t>Dr. THENNARASU P</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?hl=en&amp;user=0zYqQyAAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Thennarasu-Palani-3?ev=hdr_xprf</t>
+  </si>
+  <si>
+    <t>0000-0001-8729-4571</t>
+  </si>
+  <si>
+    <t>https://www.webofscience.com/wos/op/publications/add-suggested-publications</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/authid/detail.uri?authorId=57200900793</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/thennarasu-pa-2943b373/</t>
+  </si>
+  <si>
+    <t>VEC-002-04-155</t>
+  </si>
+  <si>
+    <t>YUVARAJ M</t>
+  </si>
+  <si>
+    <t>https://scholar.google.co.in/citations?user=ad1pYeEAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Yuvaraj_m</t>
+  </si>
+  <si>
+    <t>0000-0003-2986-5369</t>
+  </si>
+  <si>
+    <t>https://www.webofscience.com/wos/author/record/AEE-7608-2022</t>
+  </si>
+  <si>
+    <t>https://id.elsevier.com/settings/redirect?code=bUb8zbeJPiYKuGtgAFo8Anxhvm5Tiijcqr1iMtGL</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/yuvaraj-maruthu-pandian-81796943/</t>
+  </si>
+  <si>
+    <t>VEC-002-04-160</t>
+  </si>
+  <si>
+    <t>Dr. SENTHAMIL SELVAN M</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=yDeX6gQAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Senthamil-Murugan</t>
+  </si>
+  <si>
+    <t>0000-0002-3674-5798</t>
+  </si>
+  <si>
+    <t>https://www.webofscience.com/wos/author/record/LKL-3897-2024</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/authid/detail.uri?authorId=58350433000</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/dr-senthamil-selvan-murugan-01811166</t>
+  </si>
+  <si>
+    <t>VEC-002-04-167</t>
+  </si>
+  <si>
+    <t>Assistant Professor</t>
   </si>
   <si>
     <t>Associate Professor</t>
   </si>
   <si>
-    <t>/static/images/profile_photos/002/VEC-002-04-002.webp</t>
-  </si>
-  <si>
-    <t>not available</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/profile/V-Chandran?ev=hdr_xprf</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/sources.uri?zone=TopNavBar&amp;origin=searchauthorfreelookup</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/dr-v-chandran-b54505117/</t>
-  </si>
-  <si>
-    <t>VEC-002-03-168</t>
-  </si>
-  <si>
-    <t>Dr. P.Thennarasu, M.E., PhD.</t>
-  </si>
-  <si>
-    <t>Assistant Professor</t>
+    <t>Professor &amp; Head</t>
   </si>
   <si>
     <t>/static/images/profile_photos/002/VEC-002-04-155.webp</t>
   </si>
   <si>
-    <t>https://scholar.google.com/citations?hl=en&amp;user=0zYqQyAAAAAJ</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/profile/Thennarasu-Palani-3?ev=hdr_xprf</t>
-  </si>
-  <si>
-    <t>https://orcid.org/my-orcid?orcid=0000-0001-8729-4571</t>
-  </si>
-  <si>
-    <t>https://www.webofscience.com/wos/op/publications/add-suggested-publications</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/authid/detail.uri?authorId=57200900793</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/thennarasu-pa-2943b373/</t>
-  </si>
-  <si>
-    <t>VEC-002-04-155</t>
-  </si>
-  <si>
-    <t>Mr. M. Yuvaraj, M.E, (Ph.D)</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/002/VEC-002-04-160.webp</t>
   </si>
   <si>
-    <t>https://scholar.google.co.in/citations?user=ad1pYeEAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/profile/Yuvaraj_m</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0003-2986-5369</t>
-  </si>
-  <si>
-    <t>https://www.webofscience.com/wos/author/record/AEE-7608-2022</t>
-  </si>
-  <si>
-    <t>https://id.elsevier.com/settings/redirect?code=bUb8zbeJPiYKuGtgAFo8Anxhvm5Tiijcqr1iMtGL</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/yuvaraj-maruthu-pandian-81796943/</t>
-  </si>
-  <si>
-    <t>VEC-002-04-160</t>
-  </si>
-  <si>
-    <t>Dr. M.Senthamil Selvan, M.E., PhD.</t>
-  </si>
-  <si>
     <t>/static/images/profile_photos/002/VEC-002-03-167.webp</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=yDeX6gQAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/profile/Senthamil-Murugan</t>
-  </si>
-  <si>
-    <t>https://orcid.org/my-orcid?orcid=0000-0002-3674-5798</t>
-  </si>
-  <si>
-    <t>https://www.webofscience.com/wos/author/record/LKL-3897-2024</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/authid/detail.uri?authorId=58350433000</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/dr-senthamil-selvan-murugan-01811166</t>
-  </si>
-  <si>
-    <t>VEC-002-04-167</t>
-  </si>
-  <si>
-    <t>Mrs. D. S.Jemima Chandra, M.E.</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/jemima-chandra-d-s-b34586184</t>
-  </si>
-  <si>
-    <t>VEC-002-04-002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,29 +247,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -266,10 +284,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -307,71 +325,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,7 +417,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -422,11 +440,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -435,13 +453,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -451,7 +469,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -460,7 +478,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -469,7 +487,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -477,10 +495,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -545,29 +563,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="52.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="47.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="44.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,150 +615,190 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
+      <c r="B2" t="s">
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="I5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I6" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F7" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H7" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J7" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Xlsx file changes and path
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/002.xlsx
+++ b/docs/STAFF-DATA/002.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -54,12 +49,24 @@
     <t>Dr. BASKARA SETHUPATHY S</t>
   </si>
   <si>
-    <t/>
+    <t>Professor &amp; Head</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/002/VEC-002-01-567.webp</t>
+  </si>
+  <si>
+    <t>VEC-002-03-567</t>
   </si>
   <si>
     <t>Dr. CHANDRAN V</t>
   </si>
   <si>
+    <t>Associate Professor</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/002/VEC-002-03-168.webp</t>
+  </si>
+  <si>
     <t>not available</t>
   </si>
   <si>
@@ -78,6 +85,9 @@
     <t>JEMIMA CHANDRA D S</t>
   </si>
   <si>
+    <t>Assistant Professor</t>
+  </si>
+  <si>
     <t>/static/images/profile_photos/002/VEC-002-04-002.webp</t>
   </si>
   <si>
@@ -90,6 +100,9 @@
     <t>Dr. THENNARASU P</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/002/VEC-002-04-155.webp</t>
+  </si>
+  <si>
     <t>https://scholar.google.com/citations?hl=en&amp;user=0zYqQyAAAAAJ</t>
   </si>
   <si>
@@ -114,6 +127,9 @@
     <t>YUVARAJ M</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/002/VEC-002-04-160.webp</t>
+  </si>
+  <si>
     <t>https://scholar.google.co.in/citations?user=ad1pYeEAAAAJ&amp;hl=en</t>
   </si>
   <si>
@@ -138,6 +154,9 @@
     <t>Dr. SENTHAMIL SELVAN M</t>
   </si>
   <si>
+    <t>/static/images/profile_photos/002/VEC-002-03-167.webp</t>
+  </si>
+  <si>
     <t>https://scholar.google.com/citations?user=yDeX6gQAAAAJ&amp;hl=en</t>
   </si>
   <si>
@@ -157,39 +176,13 @@
   </si>
   <si>
     <t>VEC-002-04-167</t>
-  </si>
-  <si>
-    <t>Assistant Professor</t>
-  </si>
-  <si>
-    <t>Associate Professor</t>
-  </si>
-  <si>
-    <t>Professor &amp; Head</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/002/VEC-002-04-155.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/002/VEC-002-04-160.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/002/VEC-002-03-167.webp</t>
-  </si>
-  <si>
-    <t>VEC-002-03-567</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/002/VEC-002-04-567.webp</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/002/VEC-002-03-168.webp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,12 +206,10 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,41 +251,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -305,10 +293,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -346,71 +334,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,7 +426,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -461,11 +449,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -474,13 +462,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -490,7 +478,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -499,7 +487,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -508,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -516,10 +504,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -590,21 +578,23 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="52.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="47.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="44.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,196 +626,173 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exel and json changes
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/002.xlsx
+++ b/docs/STAFF-DATA/002.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE7DE50-07A8-4BD2-916C-1DF3A52857D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -88,22 +82,10 @@
     <t>VEC-002-03-168</t>
   </si>
   <si>
-    <t>JEMIMA CHANDRA D S</t>
+    <t>Dr. THENNARASU P</t>
   </si>
   <si>
     <t>Assistant Professor</t>
-  </si>
-  <si>
-    <t>/static/images/profile_photos/002/VEC-002-04-002.webp</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/jemima-chandra-d-s-b34586184</t>
-  </si>
-  <si>
-    <t>VEC-002-04-002</t>
-  </si>
-  <si>
-    <t>Dr. THENNARASU P</t>
   </si>
   <si>
     <t>/static/images/profile_photos/002/VEC-002-04-155.webp</t>
@@ -199,7 +181,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,10 +213,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -274,53 +256,42 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -331,10 +302,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -372,71 +343,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -464,7 +435,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -487,11 +458,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -500,13 +471,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -516,7 +487,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -525,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -534,7 +505,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -542,10 +513,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -610,27 +581,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="52.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="47.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="44.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,181 +635,168 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
+      <c r="E6" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+      <c r="A7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
+      <c r="B7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some insertion and major staff excel changes
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/002.xlsx
+++ b/docs/STAFF-DATA/002.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E78AB66-4D30-420C-B07B-09A353B4BFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -118,6 +112,9 @@
     <t>VEC-002-04-155</t>
   </si>
   <si>
+    <t>Mr. YUVARAJ M</t>
+  </si>
+  <si>
     <t>/static/images/profile_photos/002/VEC-002-04-160.webp</t>
   </si>
   <si>
@@ -142,6 +139,21 @@
     <t>VEC-002-04-160</t>
   </si>
   <si>
+    <t>Mr. DINESHBABU D</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/002/VEC-002-04-010.webp</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?hl=en&amp;user=BNZQRpIAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dineshbabu-d-463108128/</t>
+  </si>
+  <si>
+    <t>VEC-002-04-010</t>
+  </si>
+  <si>
     <t>Dr. SENTHAMIL SELVAN M</t>
   </si>
   <si>
@@ -169,6 +181,9 @@
     <t>VEC-002-04-167</t>
   </si>
   <si>
+    <t>Mr. BHARANI KUMAR M</t>
+  </si>
+  <si>
     <t>Lab Instructor</t>
   </si>
   <si>
@@ -176,19 +191,14 @@
   </si>
   <si>
     <t>VEC-002-05-002</t>
-  </si>
-  <si>
-    <t>Mr. YUVARAJ M</t>
-  </si>
-  <si>
-    <t>Mr. BHARANI KUMAR M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,12 +223,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -265,35 +269,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -304,10 +317,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -345,71 +358,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,7 +450,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -460,11 +473,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -473,13 +486,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -489,7 +502,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -498,7 +511,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -507,7 +520,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -515,10 +528,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -583,27 +596,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="8" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="52.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="47.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="44.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,161 +658,266 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
+      <c r="I7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>51</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+      <c r="A8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>